<commit_message>
refactorizacion de alguns servicios ej lista
</commit_message>
<xml_diff>
--- a/zServicos.xlsx
+++ b/zServicos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t>Servicio refactorizado</t>
   </si>
@@ -315,6 +315,36 @@
   </si>
   <si>
     <t>EmisionCartasPorte</t>
+  </si>
+  <si>
+    <t>EntregaMercaderiaSinFacturaElemento</t>
+  </si>
+  <si>
+    <t>EntregaMercaderiaSinFacturaConPedido</t>
+  </si>
+  <si>
+    <t>EntregaMercaderiaSinFacturaConPedidoParaExportacion</t>
+  </si>
+  <si>
+    <t>EntregaMercaderiaSinFacturaNiPedido</t>
+  </si>
+  <si>
+    <t>ListaElemento</t>
+  </si>
+  <si>
+    <t>ListaHischeq</t>
+  </si>
+  <si>
+    <t>ListaKardex</t>
+  </si>
+  <si>
+    <t>ListaMayorSalidaExcel</t>
+  </si>
+  <si>
+    <t>ListaSaldosPedidosSalidaExcel</t>
+  </si>
+  <si>
+    <t>ListaSituacionTrigoUnaFechaSalidaExcel</t>
   </si>
   <si>
     <t>servicio refacturizado</t>
@@ -354,7 +384,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
@@ -362,7 +391,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="DejaVu Sans"/>
@@ -370,7 +398,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
@@ -505,7 +532,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -575,6 +602,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -663,20 +702,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="17.9"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="48.8461538461539"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -684,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -692,115 +731,115 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>22</v>
       </c>
@@ -808,19 +847,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
       <c r="B23" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -828,25 +867,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
       <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
@@ -854,13 +893,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="13"/>
       <c r="B29" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
@@ -868,19 +907,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
       <c r="B32" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
         <v>38</v>
       </c>
@@ -888,49 +927,49 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
       <c r="B34" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
       <c r="B35" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="11"/>
       <c r="B36" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="11"/>
       <c r="B37" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
       <c r="B38" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11"/>
       <c r="B39" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="13"/>
       <c r="B40" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -938,19 +977,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>
       <c r="B43" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>51</v>
       </c>
@@ -958,91 +997,91 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11"/>
       <c r="B45" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11"/>
       <c r="B46" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11"/>
       <c r="B47" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11"/>
       <c r="B48" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11"/>
       <c r="B49" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11"/>
       <c r="B50" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11"/>
       <c r="B51" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11"/>
       <c r="B52" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="11"/>
       <c r="B53" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="11"/>
       <c r="B54" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11"/>
       <c r="B55" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="11"/>
       <c r="B56" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="11"/>
       <c r="B57" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="13"/>
       <c r="B58" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>67</v>
       </c>
@@ -1050,13 +1089,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="7"/>
       <c r="B60" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
         <v>70</v>
       </c>
@@ -1064,13 +1103,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="13"/>
       <c r="B62" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
         <v>73</v>
       </c>
@@ -1078,37 +1117,37 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="7"/>
       <c r="B68" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
         <v>80</v>
       </c>
@@ -1116,13 +1155,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="13"/>
       <c r="B70" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
         <v>83</v>
       </c>
@@ -1130,43 +1169,43 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
       <c r="B77" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="15" t="s">
         <v>91</v>
       </c>
@@ -1174,34 +1213,86 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="16"/>
       <c r="B79" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="16"/>
       <c r="B80" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="16"/>
       <c r="B81" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="16"/>
       <c r="B82" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="17"/>
       <c r="B83" s="17" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="19"/>
+      <c r="B85" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="20"/>
+      <c r="B86" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="16"/>
+      <c r="B88" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="16"/>
+      <c r="B89" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="16"/>
+      <c r="B90" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="17"/>
+      <c r="B91" s="17" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1223,57 +1314,57 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>99</v>
+      <c r="A1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
casi terminamos faltan 7
</commit_message>
<xml_diff>
--- a/zServicos.xlsx
+++ b/zServicos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="274">
   <si>
     <t xml:space="preserve">Servicio refactorizado</t>
   </si>
@@ -29,12 +29,24 @@
     <t xml:space="preserve">Operaciones refactorizadas</t>
   </si>
   <si>
+    <t xml:space="preserve">Tiempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criterio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notas</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABM Elemento</t>
   </si>
   <si>
     <t xml:space="preserve">ABMArchivoAcreedores</t>
   </si>
   <si>
+    <t xml:space="preserve">157min</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABMArchivoClientes</t>
   </si>
   <si>
@@ -89,18 +101,45 @@
     <t xml:space="preserve">ABMPedidos</t>
   </si>
   <si>
+    <t xml:space="preserve">CajaIngresosYEgresos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mismo comportamiento en las operaciones, atributos similares en los mensajes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posteriormente agregado el tiempo fue el analisis para ver si se agregaba a este grupo</t>
+  </si>
+  <si>
     <t xml:space="preserve">AltasYBajasElemento</t>
   </si>
   <si>
     <t xml:space="preserve">AltasYBajasDevolucionBolsas</t>
   </si>
   <si>
+    <t xml:space="preserve">10min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de los archivos, igualdad en las operaciones.</t>
+  </si>
+  <si>
     <t xml:space="preserve">AltasyBajasRecibosProvisoriosAnulados</t>
   </si>
   <si>
     <t xml:space="preserve">AltasYBajasTalonariosRecibosProvisoriosEnviados</t>
   </si>
   <si>
+    <t xml:space="preserve">AbuInterdepositos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posteriormente agregado el tiempo fue el analisis para ver si se agregaba a este grupo, se agregaron operaciones al servicio refactorizado pertenecientes a este servicio</t>
+  </si>
+  <si>
     <t xml:space="preserve">AnulacionElemento</t>
   </si>
   <si>
@@ -143,6 +182,12 @@
     <t xml:space="preserve">ArmadoArchivosComunicacionCartaPorteRecibidas</t>
   </si>
   <si>
+    <t xml:space="preserve">20Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre  y cantidad de servicios</t>
+  </si>
+  <si>
     <t xml:space="preserve">ArmadoCitiCompras</t>
   </si>
   <si>
@@ -164,6 +209,18 @@
     <t xml:space="preserve">ArmaRegistroRetenciones</t>
   </si>
   <si>
+    <t xml:space="preserve">ConversionPadronIngresosBrutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en los mensajes, se agregaron las operaciones del servicio al servicio refactorizado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregado posteriormente, analizando la similitud de los archivos, misma operation y atributos en los mensajes</t>
+  </si>
+  <si>
     <t xml:space="preserve">BajaElemento</t>
   </si>
   <si>
@@ -230,18 +287,48 @@
     <t xml:space="preserve">DebitosCreditosCompraCereal</t>
   </si>
   <si>
+    <t xml:space="preserve">4 Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre servicios, nombre y cantidad de operaciones</t>
+  </si>
+  <si>
     <t xml:space="preserve">DebitosCreditosVarios</t>
   </si>
   <si>
+    <t xml:space="preserve">CreditosPorDevoluciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en los mensajes se agregaron las operaciones al servicio refactorizado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NotaDeCreditoSinRemitoConPedidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4Min</t>
+  </si>
+  <si>
     <t xml:space="preserve">VentasPorZonaSubproductoMesSalida</t>
   </si>
   <si>
     <t xml:space="preserve">VentasPorZonaSubproductoMesSalidaExcel</t>
   </si>
   <si>
+    <t xml:space="preserve">7 min</t>
+  </si>
+  <si>
     <t xml:space="preserve">VentasPorZonaSubproductoMesSalidaExcelDetalle</t>
   </si>
   <si>
+    <t xml:space="preserve">DescuentosConcedidosPorZonasMesSalidaExcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mismo comportamiento en </t>
+  </si>
+  <si>
     <t xml:space="preserve">ControlElemento</t>
   </si>
   <si>
@@ -302,6 +389,9 @@
     <t xml:space="preserve">EmisionRecibosCobroDeudores</t>
   </si>
   <si>
+    <t xml:space="preserve">25min</t>
+  </si>
+  <si>
     <t xml:space="preserve">EmisionRecibos</t>
   </si>
   <si>
@@ -317,6 +407,12 @@
     <t xml:space="preserve">EmisionCartasPorte</t>
   </si>
   <si>
+    <t xml:space="preserve">ComplementoAlEmisorRecibos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en los elemento, se agregaron las operaciones de este servicio al servicio refactorizado.</t>
+  </si>
+  <si>
     <t xml:space="preserve">EntregaMercaderiaSinFacturaElemento</t>
   </si>
   <si>
@@ -413,6 +509,9 @@
     <t xml:space="preserve">ImpresionCuentasOtrosDeudores</t>
   </si>
   <si>
+    <t xml:space="preserve">16Min</t>
+  </si>
+  <si>
     <t xml:space="preserve">ImpresionFacturaCredito</t>
   </si>
   <si>
@@ -428,24 +527,51 @@
     <t xml:space="preserve">ImpresionTotalesMovimientosStockMensual</t>
   </si>
   <si>
+    <t xml:space="preserve">DetalleRetencionesLibroOrdenesPago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregado posteriormente, similitud de las operaciones y los mensajes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DuplicadoOrdenesPagoYComprobanteRetenciones</t>
+  </si>
+  <si>
     <t xml:space="preserve">ImpresorElemento</t>
   </si>
   <si>
     <t xml:space="preserve">ImpresorCarteraDocumentosACobrar</t>
   </si>
   <si>
+    <t xml:space="preserve">9Min</t>
+  </si>
+  <si>
     <t xml:space="preserve">ImpresorPreciosPromedios</t>
   </si>
   <si>
     <t xml:space="preserve">ImpresorPreciosPromediosTrigo</t>
   </si>
   <si>
+    <t xml:space="preserve">ImpresionCarteraInterdepositos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11min</t>
+  </si>
+  <si>
     <t xml:space="preserve">ListadoElemento</t>
   </si>
   <si>
     <t xml:space="preserve">ListadoChequesRecibidosSalidaExcel</t>
   </si>
   <si>
+    <t xml:space="preserve">54min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de los wsdl, nombre de las operaciones, cantidad de operaciones, similitud en el comportamiento de las operaciones. </t>
+  </si>
+  <si>
     <t xml:space="preserve">ListadoChequesRecibidos</t>
   </si>
   <si>
@@ -491,6 +617,18 @@
     <t xml:space="preserve">ListadoHarinaVendida</t>
   </si>
   <si>
+    <t xml:space="preserve">ChequesAFechaPorZonaMes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en los mensajes y el comportamiento de las operaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListaContabilizaBorraCaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7min</t>
+  </si>
+  <si>
     <t xml:space="preserve">LibroVentas</t>
   </si>
   <si>
@@ -548,6 +686,12 @@
     <t xml:space="preserve">ListadorDeudasChequesRechazadosCartaConvalidando</t>
   </si>
   <si>
+    <t xml:space="preserve">17min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en el comportamiento de las operaciones tambien en el nombre de los servicios</t>
+  </si>
+  <si>
     <t xml:space="preserve">ListadorDeudasChequesRechazadosCartaReclamo</t>
   </si>
   <si>
@@ -569,6 +713,12 @@
     <t xml:space="preserve">ListadorDeudasUnCliente</t>
   </si>
   <si>
+    <t xml:space="preserve">DeudasPorPantalla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregado posteriormente,mismas operaciones y los mensajes.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ListadorEstadisticas</t>
   </si>
   <si>
@@ -597,6 +747,96 @@
   </si>
   <si>
     <t xml:space="preserve">ListadorNuevoLibroRecibos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadoVeintePrimerosDeudoresAcreedoresProveedores </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadoVeintePrimerosDeudoresAcreedoresProveedores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en el nombre de los servicios y las operaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadoVeintePrimerosDeudoresAcreedoresProveedoresSalidaExcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeudoresQueExcedenTope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Misma operación, similitud en los mensajes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MercaderiaAEntregar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MercaderiaAEntregarPorZona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MercaderiaAEntregarPorZonaSalidaExcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsultaListaMercaderiaAEntregar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModificacionesElemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModificacionesComisiones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModificacionesArrastreCaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PedidosPendientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PedidosPendientesPorArticuloCliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de las operaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PedidosPendientesPorZonaSalidaExcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadorElemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadorMovimientosCuentasAcreedoresPorVencimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadorPercepcionesLibroIva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadoTotalesLibroIvaCompras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListadoTotalesCobranzaMensual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BusquedaMovimientosRepetidosMercaderiaAEntregar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similitud en el comportamiento de las operaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MovimientoCliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12Min</t>
   </si>
   <si>
     <t xml:space="preserve">servicio refacturizado</t>
@@ -718,21 +958,7 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
-      <right style="hair"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="hair"/>
       <top/>
       <bottom/>
@@ -743,6 +969,20 @@
       <right style="hair"/>
       <top/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -803,15 +1043,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -827,7 +1059,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -843,11 +1083,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -855,11 +1099,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -867,15 +1107,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -964,17 +1204,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B164"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A150" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A159" activeCellId="0" sqref="A159"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.9878542510121"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -984,1041 +1226,1455 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
-        <v>7</v>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
-        <v>13</v>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="s">
-        <v>15</v>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
-        <v>16</v>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>17</v>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
-        <v>18</v>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
-        <v>19</v>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
-        <v>20</v>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
-        <v>21</v>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>23</v>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12" t="s">
-        <v>24</v>
+      <c r="A22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14" t="s">
-        <v>25</v>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>27</v>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6" t="s">
-        <v>29</v>
+      <c r="A26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8" t="s">
-        <v>30</v>
+      <c r="A27" s="4"/>
+      <c r="B27" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>32</v>
+      <c r="A28" s="4"/>
+      <c r="B28" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14" t="s">
-        <v>33</v>
+      <c r="A29" s="5"/>
+      <c r="B29" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>35</v>
+      <c r="A30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
-        <v>36</v>
+      <c r="A31" s="9"/>
+      <c r="B31" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
-        <v>37</v>
+      <c r="A32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>39</v>
+      <c r="A33" s="4"/>
+      <c r="B33" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11" t="s">
-        <v>40</v>
+      <c r="A34" s="5"/>
+      <c r="B34" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11" t="s">
-        <v>41</v>
+      <c r="A35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11" t="s">
-        <v>42</v>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11" t="s">
-        <v>43</v>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11" t="s">
-        <v>44</v>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11" t="s">
-        <v>45</v>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13" t="s">
-        <v>46</v>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>48</v>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5" t="s">
-        <v>49</v>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7" t="s">
-        <v>50</v>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>52</v>
+      <c r="A44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11" t="s">
-        <v>53</v>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11" t="s">
-        <v>54</v>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11" t="s">
-        <v>55</v>
+      <c r="A47" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11" t="s">
-        <v>56</v>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11" t="s">
-        <v>57</v>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11" t="s">
-        <v>58</v>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11" t="s">
-        <v>59</v>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11" t="s">
-        <v>60</v>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11" t="s">
-        <v>61</v>
+      <c r="A53" s="8"/>
+      <c r="B53" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11" t="s">
-        <v>62</v>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11" t="s">
-        <v>63</v>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11" t="s">
-        <v>64</v>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11" t="s">
-        <v>65</v>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13" t="s">
-        <v>66</v>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>68</v>
+      <c r="A59" s="8"/>
+      <c r="B59" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7" t="s">
-        <v>69</v>
+      <c r="A60" s="8"/>
+      <c r="B60" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="A61" s="9"/>
       <c r="B61" s="9" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13" t="s">
-        <v>72</v>
+      <c r="A62" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>74</v>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5" t="s">
-        <v>75</v>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
-        <v>76</v>
+        <v>94</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5" t="s">
-        <v>77</v>
+      <c r="A66" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5" t="s">
-        <v>78</v>
+      <c r="A67" s="8"/>
+      <c r="B67" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7" t="s">
-        <v>79</v>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>81</v>
+      <c r="A69" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13" t="s">
-        <v>82</v>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>84</v>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5" t="s">
-        <v>85</v>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5" t="s">
-        <v>86</v>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5" t="s">
-        <v>88</v>
+      <c r="A75" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5" t="s">
-        <v>89</v>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7" t="s">
-        <v>90</v>
+      <c r="A77" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>92</v>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="16"/>
-      <c r="B79" s="16" t="s">
-        <v>93</v>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="16"/>
-      <c r="B80" s="16" t="s">
-        <v>94</v>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="16"/>
-      <c r="B81" s="16" t="s">
-        <v>95</v>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="16"/>
-      <c r="B82" s="16" t="s">
-        <v>96</v>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="17"/>
-      <c r="B83" s="17" t="s">
-        <v>97</v>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>99</v>
+      <c r="A84" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="19"/>
-      <c r="B85" s="19" t="s">
-        <v>100</v>
-      </c>
+      <c r="A85" s="16"/>
+      <c r="B85" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" s="17"/>
     </row>
     <row r="86" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20" t="s">
-        <v>101</v>
+      <c r="A86" s="16"/>
+      <c r="B86" s="16" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B87" s="15" t="s">
-        <v>103</v>
+      <c r="A87" s="16"/>
+      <c r="B87" s="16" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="16"/>
       <c r="B88" s="16" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="16"/>
       <c r="B89" s="16" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="16"/>
-      <c r="B90" s="16" t="s">
-        <v>106</v>
+      <c r="A90" s="18"/>
+      <c r="B90" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="17"/>
-      <c r="B91" s="17" t="s">
-        <v>107</v>
+      <c r="A91" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B92" s="21" t="s">
-        <v>109</v>
+      <c r="A92" s="20"/>
+      <c r="B92" s="20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="22"/>
-      <c r="B93" s="22" t="s">
-        <v>110</v>
+      <c r="A93" s="6"/>
+      <c r="B93" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22" t="s">
-        <v>111</v>
+      <c r="A94" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="22"/>
-      <c r="B95" s="22" t="s">
-        <v>112</v>
+      <c r="A95" s="16"/>
+      <c r="B95" s="16" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="22"/>
-      <c r="B96" s="22" t="s">
-        <v>113</v>
+      <c r="A96" s="16"/>
+      <c r="B96" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="22"/>
-      <c r="B97" s="22" t="s">
-        <v>114</v>
+      <c r="A97" s="16"/>
+      <c r="B97" s="16" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="23"/>
-      <c r="B98" s="23" t="s">
-        <v>115</v>
+      <c r="A98" s="18"/>
+      <c r="B98" s="18" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B99" s="15" t="s">
-        <v>117</v>
+      <c r="A99" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="16"/>
-      <c r="B100" s="16" t="s">
-        <v>118</v>
+      <c r="A100" s="22"/>
+      <c r="B100" s="22" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="16"/>
-      <c r="B101" s="16" t="s">
-        <v>119</v>
+      <c r="A101" s="22"/>
+      <c r="B101" s="22" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="16"/>
-      <c r="B102" s="16" t="s">
-        <v>120</v>
+      <c r="A102" s="22"/>
+      <c r="B102" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="16"/>
-      <c r="B103" s="16" t="s">
-        <v>121</v>
+      <c r="A103" s="22"/>
+      <c r="B103" s="22" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="16"/>
-      <c r="B104" s="16" t="s">
-        <v>122</v>
+      <c r="A104" s="22"/>
+      <c r="B104" s="22" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="16"/>
-      <c r="B105" s="16" t="s">
-        <v>123</v>
+      <c r="A105" s="23"/>
+      <c r="B105" s="23" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17" t="s">
-        <v>124</v>
+      <c r="A106" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B107" s="18" t="s">
-        <v>126</v>
+      <c r="A107" s="16"/>
+      <c r="B107" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="20"/>
-      <c r="B108" s="20" t="s">
-        <v>127</v>
+      <c r="A108" s="16"/>
+      <c r="B108" s="16" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>129</v>
+      <c r="A109" s="16"/>
+      <c r="B109" s="16" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="16"/>
       <c r="B110" s="16" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="16"/>
       <c r="B111" s="16" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="24"/>
+      <c r="A112" s="16"/>
       <c r="B112" s="16" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="16"/>
-      <c r="B113" s="16" t="s">
-        <v>133</v>
+      <c r="A113" s="18"/>
+      <c r="B113" s="18" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="17"/>
-      <c r="B114" s="17" t="s">
-        <v>134</v>
+      <c r="A114" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B115" s="18" t="s">
-        <v>136</v>
+      <c r="A115" s="6"/>
+      <c r="B115" s="6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="19"/>
-      <c r="B116" s="19" t="s">
-        <v>137</v>
+      <c r="A116" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="20"/>
-      <c r="B117" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B118" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="16"/>
+      <c r="A117" s="16"/>
+      <c r="B117" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="16"/>
+      <c r="B118" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="24"/>
       <c r="B119" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="16"/>
       <c r="B120" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="16"/>
       <c r="B121" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="16"/>
       <c r="B122" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D122" s="0"/>
+      <c r="E122" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="16"/>
       <c r="B123" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="16"/>
-      <c r="B124" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="16"/>
-      <c r="B125" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="16"/>
-      <c r="B126" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="16"/>
-      <c r="B127" s="16" t="s">
-        <v>149</v>
+        <v>171</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D123" s="0"/>
+      <c r="E123" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B124" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A125" s="20"/>
+      <c r="B125" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A126" s="20"/>
+      <c r="B126" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A127" s="19"/>
+      <c r="B127" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="16"/>
+      <c r="A128" s="16" t="s">
+        <v>179</v>
+      </c>
       <c r="B128" s="16" t="s">
-        <v>150</v>
+        <v>180</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="16"/>
       <c r="B129" s="16" t="s">
-        <v>151</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D129" s="17"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="16"/>
       <c r="B130" s="16" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="16"/>
       <c r="B131" s="16" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="16"/>
       <c r="B132" s="16" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="17"/>
-      <c r="B133" s="17" t="s">
-        <v>155</v>
+      <c r="A133" s="16"/>
+      <c r="B133" s="16" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B134" s="18" t="s">
-        <v>157</v>
+      <c r="A134" s="16"/>
+      <c r="B134" s="16" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="19"/>
-      <c r="B135" s="19" t="s">
-        <v>158</v>
+      <c r="A135" s="16"/>
+      <c r="B135" s="16" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="20"/>
-      <c r="B136" s="20" t="s">
-        <v>159</v>
+      <c r="A136" s="16"/>
+      <c r="B136" s="16" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B137" s="15" t="s">
-        <v>161</v>
+      <c r="A137" s="16"/>
+      <c r="B137" s="16" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="16"/>
       <c r="B138" s="16" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="16"/>
       <c r="B139" s="16" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="16"/>
       <c r="B140" s="16" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="16"/>
       <c r="B141" s="16" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="16"/>
       <c r="B142" s="16" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="17"/>
-      <c r="B143" s="17" t="s">
-        <v>167</v>
+      <c r="A143" s="16"/>
+      <c r="B143" s="16" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B144" s="18" t="s">
-        <v>169</v>
+      <c r="A144" s="16"/>
+      <c r="B144" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="19"/>
-      <c r="B145" s="19" t="s">
-        <v>170</v>
+      <c r="A145" s="18"/>
+      <c r="B145" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="19"/>
+      <c r="A146" s="19" t="s">
+        <v>202</v>
+      </c>
       <c r="B146" s="19" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B148" s="15" t="s">
-        <v>174</v>
+      <c r="A148" s="6"/>
+      <c r="B148" s="6" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="16"/>
-      <c r="B149" s="16" t="s">
-        <v>175</v>
+      <c r="A149" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B149" s="15" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="16"/>
       <c r="B150" s="16" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="16"/>
       <c r="B151" s="16" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="16"/>
       <c r="B152" s="16" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="16"/>
       <c r="B153" s="16" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="16"/>
       <c r="B154" s="16" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="16"/>
-      <c r="B155" s="16" t="s">
-        <v>180</v>
+      <c r="A155" s="18"/>
+      <c r="B155" s="18" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="17"/>
-      <c r="B156" s="17" t="s">
-        <v>181</v>
+      <c r="A156" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B156" s="19" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="B157" s="18" t="s">
-        <v>182</v>
+      <c r="A157" s="20"/>
+      <c r="B157" s="20" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="B159" s="15" t="s">
-        <v>185</v>
+      <c r="A159" s="6"/>
+      <c r="B159" s="6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="16"/>
-      <c r="B160" s="16" t="s">
-        <v>186</v>
+      <c r="A160" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B160" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="16"/>
       <c r="B161" s="16" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="17"/>
-      <c r="B162" s="17" t="s">
-        <v>188</v>
+      <c r="A162" s="16"/>
+      <c r="B162" s="16" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="B163" s="18" t="s">
-        <v>190</v>
+      <c r="A163" s="16"/>
+      <c r="B163" s="16" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="20"/>
-      <c r="B164" s="20" t="s">
-        <v>191</v>
+      <c r="A164" s="16"/>
+      <c r="B164" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="16"/>
+      <c r="B165" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="16"/>
+      <c r="B166" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="16"/>
+      <c r="B167" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="16"/>
+      <c r="B168" s="16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="18"/>
+      <c r="B169" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B170" s="19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="6"/>
+      <c r="B171" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B172" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="16"/>
+      <c r="B173" s="16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="16"/>
+      <c r="B174" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="18"/>
+      <c r="B175" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B176" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="6"/>
+      <c r="B177" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B178" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="16"/>
+      <c r="B179" s="16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="18"/>
+      <c r="B180" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="B181" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="20"/>
+      <c r="B182" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="6"/>
+      <c r="B183" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B184" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="18"/>
+      <c r="B185" s="18" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B186" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="6"/>
+      <c r="B187" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C187" s="0"/>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B188" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="16"/>
+      <c r="B189" s="16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="16"/>
+      <c r="B190" s="16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="16"/>
+      <c r="B191" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="16"/>
+      <c r="B192" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="18"/>
+      <c r="B193" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2050,48 +2706,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>192</v>
+        <v>272</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26"/>
       <c r="B3" s="26" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26"/>
       <c r="B4" s="26" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26"/>
       <c r="B5" s="26" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26"/>
       <c r="B6" s="26" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>